<commit_message>
added second test in edit account test
</commit_message>
<xml_diff>
--- a/resources/TestData/TestData.xlsx
+++ b/resources/TestData/TestData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29113"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA32DF9D-EE79-4AF4-96A6-9ED8C17F79AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8336721-EE4D-4106-89BE-5867033ECEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="AddToCart" sheetId="4" r:id="rId2"/>
-    <sheet name="ProductDetails" sheetId="2" r:id="rId3"/>
-    <sheet name="RegistrationDetails" sheetId="3" r:id="rId4"/>
+    <sheet name="EditAccount" sheetId="5" r:id="rId3"/>
+    <sheet name="ProductDetails" sheetId="2" r:id="rId4"/>
+    <sheet name="RegistrationDetails" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -230,6 +231,18 @@
       </rPr>
       <t>cart!</t>
     </r>
+  </si>
+  <si>
+    <t>emailLogin</t>
+  </si>
+  <si>
+    <t>passwordLogin</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>alwande@gmail.com</t>
   </si>
   <si>
     <t>itemPrice</t>
@@ -245,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +285,20 @@
       <name val="Consolas"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,10 +317,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -301,8 +329,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BE2ECC-75E6-41A5-AC15-275563B4581F}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -723,6 +754,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935875CD-3714-4C95-903D-5CE5617916CF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" s="5">
+        <v>676409898</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67D9ADC9-2FCF-4DB8-B169-4A3CFFF7D629}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE39DDD9-434E-4E2F-B593-CBEAB17211FE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -744,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -763,7 +839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69A27FA-2B2D-4FA6-BAF0-BC25DDDC39DE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -781,13 +857,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>